<commit_message>
Agrego ejercicios de la practica 4, 5 y 6
</commit_message>
<xml_diff>
--- a/Practica4/ejercicio6y7.xlsx
+++ b/Practica4/ejercicio6y7.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="29">
   <si>
     <t>Proceso</t>
   </si>
@@ -88,14 +88,37 @@
     <t>Q=6</t>
   </si>
   <si>
+    <t>d) La conclusion que se puede sacar a cerca del valor del quantum es que si el mismo es demasiado grande, el algoritmo se torna parecido al FCFS.</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t>e) Usaria un valor de quantum alto en los casos donde los procesos requieran mucha CPU</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> La ventaja seria que reduciria el overhead de context sqitch y la desventaja seria que corre el riesgo de convertirse en un algoritmo parecito al FCFS.</t>
+    </r>
+  </si>
+  <si>
     <t>SRTF</t>
+  </si>
+  <si>
+    <t>b) La ventaja que noto es que se redujo el TPR y TPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -116,6 +139,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -152,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -164,6 +191,12 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1934,6 +1967,16 @@
         <v>5.6</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="53">
       <c r="A53" s="1" t="s">
         <v>0</v>
@@ -2266,7 +2309,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="1"/>
@@ -2314,7 +2357,15 @@
         <v>3.6</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A41"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrego hasta el ejercicio 13 de la practica 4 y corrijo el 7 en la practica 5
</commit_message>
<xml_diff>
--- a/Practica4/ejercicio6y7.xlsx
+++ b/Practica4/ejercicio6y7.xlsx
@@ -1074,23 +1074,23 @@
         <v>9</v>
       </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>2.0</v>
-      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="O15" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="P15" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="Q15" s="1" t="s">
+        <v>2.0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
@@ -1099,10 +1099,10 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="1">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="AB15" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="16">
@@ -1125,18 +1125,16 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N16" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
@@ -1145,10 +1143,10 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="1">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="AB16" s="1">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
@@ -1194,11 +1192,11 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2">
         <f t="shared" ref="AA17:AB17" si="2">average(AA12:AA16)</f>
-        <v>8.4</v>
+        <v>7.8</v>
       </c>
       <c r="AB17" s="2">
         <f t="shared" si="2"/>
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="21">

</xml_diff>